<commit_message>
psy 2021 : modalité de réalisation de l'acte ambulatoire (vidéo, audio, présentiel)
</commit_message>
<xml_diff>
--- a/formats/excel/Formats R3A 21.xlsx
+++ b/formats/excel/Formats R3A 21.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10404"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumepressiat/Documents/Developpements/Github/formats_pmeasyr/formats/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C5CA9B-8BFF-5647-AF07-93ED63D583BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A3DB52-A757-7B4F-B633-1C6A669C8241}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="460" windowWidth="27340" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
   <si>
     <t>libelle</t>
   </si>
@@ -216,13 +216,19 @@
   </si>
   <si>
     <t>DATEACTE</t>
+  </si>
+  <si>
+    <t>Modalité de réalisation de l'acte</t>
+  </si>
+  <si>
+    <t>MODREALACT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,8 +248,19 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,6 +270,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -284,10 +307,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" activeCellId="1" sqref="G1:H1048576 B21"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1004,20 +1033,20 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21">
+      <c r="A21" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="4">
         <v>1</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="4">
         <v>125</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="4">
         <v>125</v>
       </c>
       <c r="E21" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="F21" t="s">
         <v>8</v>
@@ -1025,7 +1054,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -1037,15 +1066,15 @@
         <v>126</v>
       </c>
       <c r="E22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F22" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1057,15 +1086,15 @@
         <v>127</v>
       </c>
       <c r="E23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F23" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1077,15 +1106,15 @@
         <v>128</v>
       </c>
       <c r="E24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F24" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>47</v>
+      <c r="A25" t="s">
+        <v>45</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1096,28 +1125,28 @@
       <c r="D25">
         <v>129</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>48</v>
+      <c r="E25" t="s">
+        <v>46</v>
       </c>
       <c r="F25" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>49</v>
+      <c r="A26" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="B26">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C26">
         <v>130</v>
       </c>
       <c r="D26">
-        <v>135</v>
-      </c>
-      <c r="E26" t="s">
-        <v>50</v>
+        <v>130</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="F26" t="s">
         <v>8</v>
@@ -1125,35 +1154,55 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C27">
+        <v>131</v>
+      </c>
+      <c r="D27">
         <v>136</v>
       </c>
-      <c r="D27">
-        <v>137</v>
-      </c>
       <c r="E27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F27" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>137</v>
+      </c>
+      <c r="D28">
+        <v>138</v>
+      </c>
+      <c r="E28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>53</v>
       </c>
-      <c r="C28">
-        <v>138</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="C29">
+        <v>139</v>
+      </c>
+      <c r="E29" t="s">
         <v>54</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F29" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>